<commit_message>
Forgot to upload the updated version of Baza_clienti
</commit_message>
<xml_diff>
--- a/Data/Baza_clienti.xlsx
+++ b/Data/Baza_clienti.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BTRPA\proiectu\BlankProcess\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <x:bookViews>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
+    </x:ext>
     <x:ext xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -28,116 +29,127 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </x:ext>
-  </extLst>
-</workbook>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Nume_client</t>
-  </si>
-  <si>
-    <t>CUI</t>
-  </si>
-  <si>
-    <t>Nr_factura</t>
-  </si>
-  <si>
-    <t>Data_factura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cod_Produs </t>
-  </si>
-  <si>
-    <t>Valoare_factura</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SC romprest srl</t>
-  </si>
-  <si>
-    <t>10.10.2021</t>
-  </si>
-  <si>
-    <t>SC GRM SRL</t>
-  </si>
-  <si>
-    <t>15.09.2021</t>
-  </si>
-  <si>
-    <t>SC TESSA SRL</t>
-  </si>
-  <si>
-    <t>01.10.2021</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <x:si>
+    <x:t>Nume_client</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CUI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nr_factura</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Data_factura</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cod_Produs </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Valoare_factura</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> SC romprest srl</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10.10.2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SC GRM SRL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15.09.2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SC TESSA SRL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01.10.2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>45234</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="3" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:sz val="10"/>
+      <x:color theme="1"/>
+      <x:name val="Arial"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <x:alignment vertical="center"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -436,101 +448,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>13213413</v>
-      </c>
-      <c r="C2">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>56345676</v>
-      </c>
-      <c r="C3">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>98766669</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1">
-        <v>1800</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000Clasificare BT: Uz Intern</oddFooter>
-  </headerFooter>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F4"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="E8" sqref="E8"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:cols>
+    <x:col min="1" max="2" width="16.179688" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="17.363281" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="18.726562" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="16.363281" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="16.726562" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <x:c r="A2" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="n">
+        <x:v>13213413</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="n">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E2" s="1" t="s"/>
+      <x:c r="F2" s="1" t="n">
+        <x:v>1000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <x:c r="A3" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="n">
+        <x:v>56345676</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="n">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E3" s="1" t="s"/>
+      <x:c r="F3" s="1" t="n">
+        <x:v>2400</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <x:c r="A4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="n">
+        <x:v>98766669</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="E4" s="1" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="F4" s="1" t="n">
+        <x:v>1800</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="9" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:headerFooter differentOddEven="0" differentFirst="0" scaleWithDoc="1" alignWithMargins="1">
+    <x:oddHeader/>
+    <x:oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000Clasificare BT: Uz Intern</x:oddFooter>
+    <x:evenHeader/>
+    <x:evenFooter/>
+    <x:firstHeader/>
+    <x:firstFooter/>
+  </x:headerFooter>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>